<commit_message>
changing BBIP rules and update gitignore
</commit_message>
<xml_diff>
--- a/arquivos/facilidades_tecnologia_prioridade.xlsx
+++ b/arquivos/facilidades_tecnologia_prioridade.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F257064\Documents\Codes\atualizacao automacao lote\AUTMACAO_LOTE\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4E86A5-4F96-43EA-993C-A2681868D540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1425E2-A492-495C-ABE5-F6B11C30A6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>